<commit_message>
Consolidando tacticas y vista
Escribiendo las tacticas y vistas que decidimos que ibamos a utilizar en
el documento de arquitectura y actualizando mi task y log.
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/20095495.xlsx
+++ b/tspi/ciclo-2/20095495.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="2"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
     <sheet name="task" sheetId="2" r:id="rId2"/>
     <sheet name="logt" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -161,16 +166,22 @@
   <si>
     <t>Elaborar el reporte de cierre del ciclo #2 de TSPi.</t>
   </si>
+  <si>
+    <t>Consolidando las tácticas y vistas que vamos a utilizar en el documento de arquitectura.</t>
+  </si>
+  <si>
+    <t>4 y 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -247,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -316,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,11 +404,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -436,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,9 +490,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,6 +525,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -677,14 +701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALY23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="7" customWidth="1"/>
@@ -696,7 +720,7 @@
     <col min="1014" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1013" s="3" customFormat="1" ht="42.75">
+    <row r="1" spans="1:1013" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1013" ht="25.5">
+    <row r="2" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>24</v>
       </c>
@@ -1769,7 +1793,7 @@
       <c r="ALX2" s="4"/>
       <c r="ALY2" s="4"/>
     </row>
-    <row r="3" spans="1:1013" ht="25.5">
+    <row r="3" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>25</v>
       </c>
@@ -2806,7 +2830,7 @@
       <c r="ALX3" s="4"/>
       <c r="ALY3" s="4"/>
     </row>
-    <row r="4" spans="1:1013">
+    <row r="4" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>26</v>
       </c>
@@ -3843,7 +3867,7 @@
       <c r="ALX4" s="4"/>
       <c r="ALY4" s="4"/>
     </row>
-    <row r="5" spans="1:1013" ht="25.5">
+    <row r="5" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>27</v>
       </c>
@@ -4880,7 +4904,7 @@
       <c r="ALX5" s="4"/>
       <c r="ALY5" s="4"/>
     </row>
-    <row r="6" spans="1:1013" ht="38.25">
+    <row r="6" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>28</v>
       </c>
@@ -5917,7 +5941,7 @@
       <c r="ALX6" s="4"/>
       <c r="ALY6" s="4"/>
     </row>
-    <row r="7" spans="1:1013" ht="25.5">
+    <row r="7" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>29</v>
       </c>
@@ -6954,7 +6978,7 @@
       <c r="ALX7" s="4"/>
       <c r="ALY7" s="4"/>
     </row>
-    <row r="8" spans="1:1013">
+    <row r="8" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>30</v>
       </c>
@@ -7991,7 +8015,7 @@
       <c r="ALX8" s="4"/>
       <c r="ALY8" s="4"/>
     </row>
-    <row r="9" spans="1:1013" ht="25.5">
+    <row r="9" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>31</v>
       </c>
@@ -9028,7 +9052,7 @@
       <c r="ALX9" s="4"/>
       <c r="ALY9" s="4"/>
     </row>
-    <row r="10" spans="1:1013" ht="25.5">
+    <row r="10" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>32</v>
       </c>
@@ -10065,7 +10089,7 @@
       <c r="ALX10" s="4"/>
       <c r="ALY10" s="4"/>
     </row>
-    <row r="11" spans="1:1013" ht="25.5">
+    <row r="11" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>33</v>
       </c>
@@ -11102,7 +11126,7 @@
       <c r="ALX11" s="4"/>
       <c r="ALY11" s="4"/>
     </row>
-    <row r="12" spans="1:1013" ht="25.5">
+    <row r="12" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>34</v>
       </c>
@@ -12139,7 +12163,7 @@
       <c r="ALX12" s="4"/>
       <c r="ALY12" s="4"/>
     </row>
-    <row r="13" spans="1:1013" ht="25.5">
+    <row r="13" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>35</v>
       </c>
@@ -13176,7 +13200,7 @@
       <c r="ALX13" s="4"/>
       <c r="ALY13" s="4"/>
     </row>
-    <row r="14" spans="1:1013" ht="25.5">
+    <row r="14" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>36</v>
       </c>
@@ -14213,7 +14237,7 @@
       <c r="ALX14" s="4"/>
       <c r="ALY14" s="4"/>
     </row>
-    <row r="15" spans="1:1013" ht="25.5">
+    <row r="15" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>37</v>
       </c>
@@ -15250,7 +15274,7 @@
       <c r="ALX15" s="4"/>
       <c r="ALY15" s="4"/>
     </row>
-    <row r="16" spans="1:1013" ht="25.5">
+    <row r="16" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>38</v>
       </c>
@@ -16287,7 +16311,7 @@
       <c r="ALX16" s="4"/>
       <c r="ALY16" s="4"/>
     </row>
-    <row r="17" spans="1:1013" ht="25.5">
+    <row r="17" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>39</v>
       </c>
@@ -17324,7 +17348,7 @@
       <c r="ALX17" s="4"/>
       <c r="ALY17" s="4"/>
     </row>
-    <row r="18" spans="1:1013" ht="25.5">
+    <row r="18" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>40</v>
       </c>
@@ -17359,7 +17383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1013">
+    <row r="19" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>41</v>
       </c>
@@ -17394,7 +17418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:1013" ht="25.5">
+    <row r="20" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>42</v>
       </c>
@@ -17429,7 +17453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1013">
+    <row r="21" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43</v>
       </c>
@@ -17464,7 +17488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1013">
+    <row r="22" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>44</v>
       </c>
@@ -17499,7 +17523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1013" ht="25.5">
+    <row r="23" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>45</v>
       </c>
@@ -17545,14 +17569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" style="5"/>
@@ -17560,7 +17584,7 @@
     <col min="1025" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75" customHeight="1">
+    <row r="1" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17571,7 +17595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>24</v>
       </c>
@@ -17583,7 +17607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>25</v>
       </c>
@@ -17595,7 +17619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>28</v>
       </c>
@@ -17607,7 +17631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="12" customFormat="1">
+    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
         <v>30</v>
       </c>
@@ -17619,7 +17643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>32</v>
       </c>
@@ -17631,7 +17655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>35</v>
       </c>
@@ -17643,90 +17667,97 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="12" customFormat="1">
-      <c r="A8" s="31">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4">
+        <f>126/60</f>
+        <v>2.1</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31">
         <v>38</v>
-      </c>
-      <c r="B8" s="4">
-        <f>SUMIF(logt!$G:$G,A8,logt!$F:$F)/60</f>
-        <v>0.48333333333333334</v>
-      </c>
-      <c r="C8" s="31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4">
-        <v>41</v>
       </c>
       <c r="B9" s="4">
         <f>SUMIF(logt!$G:$G,A9,logt!$F:$F)/60</f>
-        <v>1.05</v>
-      </c>
-      <c r="C9" s="4">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C9" s="31">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4">
         <f>SUMIF(logt!$G:$G,A10,logt!$F:$F)/60</f>
-        <v>0.53333333333333333</v>
+        <v>1.05</v>
       </c>
       <c r="C10" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4">
         <f>SUMIF(logt!$G:$G,A11,logt!$F:$F)/60</f>
-        <v>1.75</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C11" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4">
         <f>SUMIF(logt!$G:$G,A12,logt!$F:$F)/60</f>
-        <v>0.95</v>
+        <v>1.75</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4">
+        <f>SUMIF(logt!$G:$G,A13,logt!$F:$F)/60</f>
+        <v>0.95</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -17739,14 +17770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="23" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="21" customWidth="1"/>
@@ -17758,7 +17789,7 @@
     <col min="9" max="16384" width="11.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.5">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
@@ -17784,7 +17815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>41924</v>
       </c>
@@ -17811,7 +17842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>41924</v>
       </c>
@@ -17838,7 +17869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>41930</v>
       </c>
@@ -17865,7 +17896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
         <v>41931</v>
       </c>
@@ -17892,7 +17923,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>41932</v>
       </c>
@@ -17919,7 +17950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>41934</v>
       </c>
@@ -17946,7 +17977,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="25.5">
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>41934</v>
       </c>
@@ -17973,7 +18004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>41936</v>
       </c>
@@ -18000,7 +18031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>41938</v>
       </c>
@@ -18027,7 +18058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25.5">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>41938</v>
       </c>
@@ -18054,7 +18085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>41938</v>
       </c>
@@ -18081,15 +18112,34 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="27"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="18"/>
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="28">
+        <v>41939</v>
+      </c>
+      <c r="B13" s="30">
+        <v>5</v>
+      </c>
+      <c r="C13" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="E13" s="22">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" ref="F13" si="1">((HOUR(D13)-HOUR(C13))*60)+(MINUTE(D13)-MINUTE(C13))-E13</f>
+        <v>13</v>
+      </c>
+      <c r="G13" s="4">
+        <v>36</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="22"/>
       <c r="C14" s="17"/>
@@ -18097,7 +18147,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="22"/>
       <c r="C15" s="17"/>
@@ -18105,7 +18155,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="22"/>
       <c r="C16" s="17"/>
@@ -18113,7 +18163,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1">
+    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24"/>
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
@@ -18123,7 +18173,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="22"/>
       <c r="C20" s="17"/>
@@ -18131,7 +18181,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="22"/>
       <c r="C21" s="17"/>
@@ -18139,7 +18189,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="22"/>
       <c r="C22" s="17"/>
@@ -18147,7 +18197,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="22"/>
       <c r="C23" s="17"/>
@@ -18155,7 +18205,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="22"/>
       <c r="C24" s="17"/>
@@ -18163,7 +18213,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="22"/>
       <c r="C25" s="17"/>
@@ -18171,7 +18221,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="22"/>
       <c r="C26" s="17"/>
@@ -18179,7 +18229,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="22"/>
       <c r="C27" s="17"/>
@@ -18187,7 +18237,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="22"/>
       <c r="C28" s="17"/>
@@ -18195,7 +18245,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="22"/>
       <c r="C29" s="17"/>
@@ -18203,7 +18253,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="18"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="22"/>
       <c r="C30" s="17"/>
@@ -18211,7 +18261,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="22"/>
       <c r="C31" s="17"/>
@@ -18219,7 +18269,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="18"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="22"/>
       <c r="C32" s="17"/>
@@ -18227,7 +18277,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="22"/>
       <c r="C33" s="17"/>
@@ -18235,7 +18285,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="18"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="22"/>
       <c r="C34" s="17"/>
@@ -18243,7 +18293,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="22"/>
       <c r="C35" s="17"/>

</xml_diff>

<commit_message>
Arreglando mi task y log
Poniendo las tareas en el ciclo que realmente se hicieron.
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/20095495.xlsx
+++ b/tspi/ciclo-2/20095495.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Id</t>
   </si>
@@ -166,12 +166,6 @@
   <si>
     <t>Elaborar el reporte de cierre del ciclo #2 de TSPi.</t>
   </si>
-  <si>
-    <t>Consolidando las tácticas y vistas que vamos a utilizar en el documento de arquitectura.</t>
-  </si>
-  <si>
-    <t>4 y 5</t>
-  </si>
 </sst>
 </file>
 
@@ -258,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -327,9 +321,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17570,10 +17561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17667,37 +17658,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>36</v>
+    <row r="8" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31">
+        <v>38</v>
       </c>
       <c r="B8" s="4">
-        <f>126/60</f>
-        <v>2.1</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>49</v>
+        <f>SUMIF(logt!$G:$G,A8,logt!$F:$F)/60</f>
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C8" s="31">
+        <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31">
-        <v>38</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>41</v>
       </c>
       <c r="B9" s="4">
         <f>SUMIF(logt!$G:$G,A9,logt!$F:$F)/60</f>
-        <v>0.48333333333333334</v>
-      </c>
-      <c r="C9" s="31">
+        <v>1.05</v>
+      </c>
+      <c r="C9" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4">
         <f>SUMIF(logt!$G:$G,A10,logt!$F:$F)/60</f>
-        <v>1.05</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C10" s="4">
         <v>5</v>
@@ -17705,11 +17696,11 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4">
         <f>SUMIF(logt!$G:$G,A11,logt!$F:$F)/60</f>
-        <v>0.53333333333333333</v>
+        <v>1.75</v>
       </c>
       <c r="C11" s="4">
         <v>5</v>
@@ -17717,27 +17708,20 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4">
         <f>SUMIF(logt!$G:$G,A12,logt!$F:$F)/60</f>
-        <v>1.75</v>
+        <v>0.95</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>45</v>
-      </c>
-      <c r="B13" s="4">
-        <f>SUMIF(logt!$G:$G,A13,logt!$F:$F)/60</f>
-        <v>0.95</v>
-      </c>
-      <c r="C13" s="4">
-        <v>5</v>
-      </c>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
@@ -17754,11 +17738,6 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -17771,10 +17750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18112,32 +18091,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="28">
-        <v>41939</v>
-      </c>
-      <c r="B13" s="30">
-        <v>5</v>
-      </c>
-      <c r="C13" s="17">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D13" s="17">
-        <v>0.67569444444444438</v>
-      </c>
-      <c r="E13" s="22">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <f t="shared" ref="F13" si="1">((HOUR(D13)-HOUR(C13))*60)+(MINUTE(D13)-MINUTE(C13))-E13</f>
-        <v>13</v>
-      </c>
-      <c r="G13" s="4">
-        <v>36</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>48</v>
-      </c>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
@@ -18155,23 +18115,23 @@
       <c r="E15" s="22"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="18"/>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="16"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="27"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
@@ -18293,14 +18253,6 @@
       <c r="E34" s="22"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="27"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="18"/>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>